<commit_message>
feat: add gpt-5 results
</commit_message>
<xml_diff>
--- a/Results/gpt-5/Upadhyaya, 36734646/cost.xlsx
+++ b/Results/gpt-5/Upadhyaya, 36734646/cost.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5877</v>
+        <v>8190</v>
       </c>
     </row>
     <row r="3">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8305</v>
+        <v>7004</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14182</v>
+        <v>15194</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.00361585</v>
+        <v>0.0802775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>